<commit_message>
few modifications made on few test cases on module att.com
</commit_message>
<xml_diff>
--- a/com.att/src/test/resources/attTestData.xlsx
+++ b/com.att/src/test/resources/attTestData.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nahid\IdeaProjects\Team5WDESeleniumBootcamp\com.att\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CCD6B9-8985-4B9F-BF87-7D1BA5D0E42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F6FCCD-B3EB-4DA0-849A-0014053E15E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{5B3D6E91-87A4-427A-B005-9C27CF189E9B}"/>
   </bookViews>
   <sheets>
     <sheet name="attSignUp" sheetId="2" r:id="rId1"/>
-    <sheet name="testInvalidSignInApproach2" sheetId="3" r:id="rId2"/>
+    <sheet name="testInvalidSignInApproach7" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>